<commit_message>
Updated all the BoS clean code
</commit_message>
<xml_diff>
--- a/BoSClean/disability_counts.xlsx
+++ b/BoSClean/disability_counts.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>Count</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -760,7 +760,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>3055</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -785,7 +785,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>3055</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>3055</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>3055</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">

</xml_diff>